<commit_message>
add script_1 section to create metadata. tsv. Add TJGIp11 input .mzML files
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00B1F25-79C5-4441-8B9D-696663185A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39458AA-2782-4C1E-83A5-A72A7256A5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1714" windowWidth="16457" windowHeight="9455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10886" yWindow="0" windowWidth="11143" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Job to Run" sheetId="2" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,23 +26,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Job Name</t>
   </si>
   <si>
-    <t>Control Folder Name</t>
-  </si>
-  <si>
     <t>Exp Folder Name</t>
   </si>
   <si>
     <t>EXP num replicates</t>
   </si>
   <si>
-    <t>Control num replicates</t>
-  </si>
-  <si>
     <t>TJGIp11</t>
   </si>
   <si>
@@ -55,6 +50,15 @@
   </si>
   <si>
     <t>TJGI2pt1_EV_gpdA</t>
+  </si>
+  <si>
+    <t>CTRL Folder Name</t>
+  </si>
+  <si>
+    <t>CTRL num replicates</t>
+  </si>
+  <si>
+    <t>Anid_HE_CTRL_TJGI2pt1_EV_gpdA_pos_2018</t>
   </si>
 </sst>
 </file>
@@ -374,11 +378,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304F4F24-DCD0-46C1-BBFB-CDC0BA63B423}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="8.921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.61328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.84375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -395,39 +461,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
update running metadata excel
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39458AA-2782-4C1E-83A5-A72A7256A5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373FF791-F61C-43ED-A394-80FD40842910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10886" yWindow="0" windowWidth="11143" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1277" windowWidth="16457" windowHeight="9454" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job to Run" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Job Name</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Anid_HE_CTRL_TJGI2pt1_EV_gpdA_pos_2018</t>
+  </si>
+  <si>
+    <t>TJGIp11_pos</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -415,7 +418,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Adjust script1 so that .mzML files (CTRL and EXP) will be stored in a single folder for a job. This change was made for downstream .MZmine jobs, where the commandline prompt needs a single folder with all relevant .mzML files.
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373FF791-F61C-43ED-A394-80FD40842910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7D64B6-DAD6-4D72-8AB6-AC544C026D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1277" windowWidth="16457" windowHeight="9454" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,20 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Job Name</t>
   </si>
   <si>
-    <t>Exp Folder Name</t>
-  </si>
-  <si>
     <t>EXP num replicates</t>
   </si>
   <si>
-    <t>TJGIp11</t>
-  </si>
-  <si>
     <t>Anid_HE_TJGIp11_pos_2018</t>
   </si>
   <si>
@@ -49,19 +43,7 @@
     <t>POS</t>
   </si>
   <si>
-    <t>TJGI2pt1_EV_gpdA</t>
-  </si>
-  <si>
-    <t>CTRL Folder Name</t>
-  </si>
-  <si>
     <t>CTRL num replicates</t>
-  </si>
-  <si>
-    <t>Anid_HE_CTRL_TJGI2pt1_EV_gpdA_pos_2018</t>
-  </si>
-  <si>
-    <t>TJGIp11_pos</t>
   </si>
 </sst>
 </file>
@@ -382,21 +364,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304F4F24-DCD0-46C1-BBFB-CDC0BA63B423}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.4609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.61328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.61328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,36 +384,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -444,22 +412,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="24.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.61328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.15234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,42 +433,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Script 1 with xml editing (incomplete) and edit import for more general filenames (edit 'Control' to 'CTRL'
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7D64B6-DAD6-4D72-8AB6-AC544C026D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAEA2B7-16B0-4BB5-9374-4ED671FFD349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1277" windowWidth="16457" windowHeight="9454" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9240" yWindow="3090" windowWidth="21600" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job to Run" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Job Name</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>CTRL num replicates</t>
+  </si>
+  <si>
+    <t>Anid_HE_TJGIp4_TMM_pos_2018</t>
   </si>
 </sst>
 </file>
@@ -367,16 +370,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,9 +393,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -412,20 +415,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.61328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -453,10 +455,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:4" s="1" customFormat="1" ht="35.6" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updates to Script 2 (not finished); copy-paste MetaboAnalyst script from Rstudio to test
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAEA2B7-16B0-4BB5-9374-4ED671FFD349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB76C9D-18CB-44F1-A1C1-C904484CCD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="3090" windowWidth="21600" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="291" yWindow="1740" windowWidth="21652" windowHeight="11126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job to Run" sheetId="2" r:id="rId1"/>
@@ -370,16 +370,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="66.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.53515625" customWidth="1"/>
+    <col min="2" max="2" width="16.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,9 +393,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -418,16 +418,16 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -455,7 +455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Functioning Script 2 with HE input data; still need to look at output and adjust output filenames
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB76C9D-18CB-44F1-A1C1-C904484CCD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F02DF0-1669-4238-AA57-A3F7E4AB9C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="291" yWindow="1740" windowWidth="21652" windowHeight="11126" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="3210" windowWidth="21555" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job to Run" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Job Name</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Anid_HE_TJGIp4_TMM_pos_2018</t>
+  </si>
+  <si>
+    <t>tutorial</t>
   </si>
 </sst>
 </file>
@@ -370,16 +373,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.53515625" customWidth="1"/>
-    <col min="2" max="2" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,7 +396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -415,19 +418,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -455,7 +458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -467,6 +470,11 @@
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script 1 specify format of .mzML input files. Add G1_MC_RCG_PNAS_pos_2021 mzML files to run example GF job.
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F02DF0-1669-4238-AA57-A3F7E4AB9C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F275537F-97BB-4DE0-8C9A-3691511DD82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="3210" windowWidth="21555" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job to Run" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Job Name</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>tutorial</t>
+  </si>
+  <si>
+    <t>G1_MC_RCG_PNAS_pos_2021</t>
   </si>
 </sst>
 </file>
@@ -373,7 +376,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,13 +401,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +480,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Script 1 fix error with deleting everyting in temp folder at start of job; added feature for specifying filename for MZmine3 batch xml template file.
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F275537F-97BB-4DE0-8C9A-3691511DD82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C101C227-4A13-4E3B-AE68-468EF6146757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>Job Name</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>G1_MC_RCG_PNAS_pos_2021</t>
+  </si>
+  <si>
+    <t>MZmine3 batch template</t>
+  </si>
+  <si>
+    <t>MZmine3_batch_params_LCMSMS_HE_for_Commandline_2024_8_test_for_Python_workflow.xml</t>
   </si>
 </sst>
 </file>
@@ -373,19 +379,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304F4F24-DCD0-46C1-BBFB-CDC0BA63B423}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,19 +404,25 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -421,10 +433,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +445,7 @@
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,8 +458,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -460,8 +475,11 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -474,13 +492,19 @@
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -492,6 +516,9 @@
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update script 1 to more GNPS input files prior to generating MetaboAnalyst input file. Add a batch params .xml file with GNPS auto-run set to 'true'; however, GNPS auto-run does not seem to work.
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C101C227-4A13-4E3B-AE68-468EF6146757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD04EB9-B702-4454-9D91-FB1F3A3807BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job to Run" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>Job Name</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>MZmine3_batch_params_LCMSMS_HE_for_Commandline_2024_8_test_for_Python_workflow.xml</t>
+  </si>
+  <si>
+    <t>MZmine3_batch_params_LCMSMS_HE_for_Commandline_2024_9_auto_GNPS_run.xml</t>
+  </si>
+  <si>
+    <t>Auto-run GNPS Job</t>
   </si>
 </sst>
 </file>
@@ -74,12 +80,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -94,11 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304F4F24-DCD0-46C1-BBFB-CDC0BA63B423}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +435,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -433,10 +446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +534,45 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add .env file to .gitignore and update Script_1_MZmine3_workflow.py to load environment variables from .env file
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD04EB9-B702-4454-9D91-FB1F3A3807BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70D4FDA-05B7-4BE8-B915-1295B39AF82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job to Run" sheetId="2" r:id="rId1"/>
@@ -394,17 +394,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304F4F24-DCD0-46C1-BBFB-CDC0BA63B423}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="66.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="66.53515625" customWidth="1"/>
+    <col min="2" max="2" width="23.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -435,7 +435,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -448,17 +448,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -492,7 +492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -509,7 +509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -517,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -534,12 +534,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -556,7 +556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Update README, add tutorial .mzML dataset (Y-p9 and Anid-TJGIp11 with EV controls), clean up Script 3 formatting
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83553B1-DAC3-4EDF-99B3-1F8213AEA21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B623F58-F9A1-4E6D-8D33-F750EA407D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="2710" windowWidth="21600" windowHeight="10950" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Multi-jobs" sheetId="1" r:id="rId1"/>
-    <sheet name="final multi-jobs (edit)" sheetId="2" r:id="rId2"/>
-    <sheet name="Need to Fix Spectra Baseline" sheetId="3" r:id="rId3"/>
-    <sheet name="All with ABMBA feat ID'd" sheetId="4" r:id="rId4"/>
+    <sheet name="Tutorial" sheetId="6" r:id="rId2"/>
+    <sheet name="final multi-jobs (edit)" sheetId="2" r:id="rId3"/>
+    <sheet name="Need to Fix Spectra Baseline" sheetId="3" r:id="rId4"/>
     <sheet name="All" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="184">
   <si>
     <t>Job Name</t>
   </si>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -976,7 +976,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -988,7 +988,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1008,7 +1008,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -1016,10 +1016,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1028,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -1036,10 +1036,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -1048,7 +1048,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -1060,10 +1060,135 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D739E2FA-5184-43EA-A577-D1F7523E554E}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" activeCellId="1" sqref="A13:XFD13 A11:XFD11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2500,7 +2625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2661,11 +2786,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F75"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" activeCellId="1" sqref="A13:XFD13 A11:XFD11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2710,1527 +2837,6 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="E27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-      <c r="E35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>100</v>
-      </c>
-      <c r="B36" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-      <c r="E36" t="s">
-        <v>102</v>
-      </c>
-      <c r="F36" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-      <c r="E37" t="s">
-        <v>105</v>
-      </c>
-      <c r="F37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B38" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s">
-        <v>107</v>
-      </c>
-      <c r="F38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>108</v>
-      </c>
-      <c r="B39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39">
-        <v>2</v>
-      </c>
-      <c r="E39" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-      <c r="E40" t="s">
-        <v>111</v>
-      </c>
-      <c r="F40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>112</v>
-      </c>
-      <c r="B41" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s">
-        <v>113</v>
-      </c>
-      <c r="F41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>116</v>
-      </c>
-      <c r="B43" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>117</v>
-      </c>
-      <c r="F43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>124</v>
-      </c>
-      <c r="B44" t="s">
-        <v>125</v>
-      </c>
-      <c r="C44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44">
-        <v>4</v>
-      </c>
-      <c r="E44" t="s">
-        <v>126</v>
-      </c>
-      <c r="F44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45">
-        <v>4</v>
-      </c>
-      <c r="E45" t="s">
-        <v>129</v>
-      </c>
-      <c r="F45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>130</v>
-      </c>
-      <c r="B46" t="s">
-        <v>125</v>
-      </c>
-      <c r="C46" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46">
-        <v>4</v>
-      </c>
-      <c r="E46" t="s">
-        <v>131</v>
-      </c>
-      <c r="F46" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>132</v>
-      </c>
-      <c r="B47" t="s">
-        <v>128</v>
-      </c>
-      <c r="C47" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47">
-        <v>4</v>
-      </c>
-      <c r="E47" t="s">
-        <v>133</v>
-      </c>
-      <c r="F47" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>134</v>
-      </c>
-      <c r="B48" t="s">
-        <v>125</v>
-      </c>
-      <c r="C48" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48">
-        <v>4</v>
-      </c>
-      <c r="E48" t="s">
-        <v>135</v>
-      </c>
-      <c r="F48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>136</v>
-      </c>
-      <c r="B49" t="s">
-        <v>128</v>
-      </c>
-      <c r="C49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49">
-        <v>4</v>
-      </c>
-      <c r="E49" t="s">
-        <v>137</v>
-      </c>
-      <c r="F49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>138</v>
-      </c>
-      <c r="B50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50">
-        <v>2</v>
-      </c>
-      <c r="E50" t="s">
-        <v>139</v>
-      </c>
-      <c r="F50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>140</v>
-      </c>
-      <c r="B51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51">
-        <v>2</v>
-      </c>
-      <c r="E51" t="s">
-        <v>141</v>
-      </c>
-      <c r="F51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>142</v>
-      </c>
-      <c r="B52" t="s">
-        <v>143</v>
-      </c>
-      <c r="C52" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52">
-        <v>2</v>
-      </c>
-      <c r="E52" t="s">
-        <v>144</v>
-      </c>
-      <c r="F52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>145</v>
-      </c>
-      <c r="B53" t="s">
-        <v>146</v>
-      </c>
-      <c r="C53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53">
-        <v>2</v>
-      </c>
-      <c r="E53" t="s">
-        <v>147</v>
-      </c>
-      <c r="F53" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>148</v>
-      </c>
-      <c r="B54" t="s">
-        <v>143</v>
-      </c>
-      <c r="C54" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54">
-        <v>2</v>
-      </c>
-      <c r="E54" t="s">
-        <v>149</v>
-      </c>
-      <c r="F54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>150</v>
-      </c>
-      <c r="B55" t="s">
-        <v>146</v>
-      </c>
-      <c r="C55" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
-      </c>
-      <c r="E55" t="s">
-        <v>151</v>
-      </c>
-      <c r="F55" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>172</v>
-      </c>
-      <c r="B56" t="s">
-        <v>173</v>
-      </c>
-      <c r="C56" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56">
-        <v>2</v>
-      </c>
-      <c r="E56" t="s">
-        <v>174</v>
-      </c>
-      <c r="F56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>152</v>
-      </c>
-      <c r="B57" t="s">
-        <v>153</v>
-      </c>
-      <c r="C57" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57">
-        <v>2</v>
-      </c>
-      <c r="E57" t="s">
-        <v>154</v>
-      </c>
-      <c r="F57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>175</v>
-      </c>
-      <c r="B58" t="s">
-        <v>173</v>
-      </c>
-      <c r="C58" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58">
-        <v>2</v>
-      </c>
-      <c r="E58" t="s">
-        <v>176</v>
-      </c>
-      <c r="F58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>155</v>
-      </c>
-      <c r="B59" t="s">
-        <v>153</v>
-      </c>
-      <c r="C59" t="s">
-        <v>13</v>
-      </c>
-      <c r="D59">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>156</v>
-      </c>
-      <c r="F59" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>177</v>
-      </c>
-      <c r="B60" t="s">
-        <v>173</v>
-      </c>
-      <c r="C60" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60">
-        <v>2</v>
-      </c>
-      <c r="E60" t="s">
-        <v>178</v>
-      </c>
-      <c r="F60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>157</v>
-      </c>
-      <c r="B61" t="s">
-        <v>153</v>
-      </c>
-      <c r="C61" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61">
-        <v>2</v>
-      </c>
-      <c r="E61" t="s">
-        <v>154</v>
-      </c>
-      <c r="F61" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>179</v>
-      </c>
-      <c r="B62" t="s">
-        <v>173</v>
-      </c>
-      <c r="C62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62">
-        <v>2</v>
-      </c>
-      <c r="E62" t="s">
-        <v>174</v>
-      </c>
-      <c r="F62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>158</v>
-      </c>
-      <c r="B63" t="s">
-        <v>153</v>
-      </c>
-      <c r="C63" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s">
-        <v>159</v>
-      </c>
-      <c r="F63" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>180</v>
-      </c>
-      <c r="B64" t="s">
-        <v>173</v>
-      </c>
-      <c r="C64" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s">
-        <v>181</v>
-      </c>
-      <c r="F64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>160</v>
-      </c>
-      <c r="B65" t="s">
-        <v>153</v>
-      </c>
-      <c r="C65" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s">
-        <v>161</v>
-      </c>
-      <c r="F65" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>182</v>
-      </c>
-      <c r="B66" t="s">
-        <v>173</v>
-      </c>
-      <c r="C66" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66">
-        <v>2</v>
-      </c>
-      <c r="E66" t="s">
-        <v>183</v>
-      </c>
-      <c r="F66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>162</v>
-      </c>
-      <c r="B67" t="s">
-        <v>153</v>
-      </c>
-      <c r="C67" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67">
-        <v>2</v>
-      </c>
-      <c r="E67" t="s">
-        <v>163</v>
-      </c>
-      <c r="F67" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>164</v>
-      </c>
-      <c r="B68" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68">
-        <v>2</v>
-      </c>
-      <c r="E68" t="s">
-        <v>165</v>
-      </c>
-      <c r="F68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>166</v>
-      </c>
-      <c r="B69" t="s">
-        <v>12</v>
-      </c>
-      <c r="C69" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69">
-        <v>2</v>
-      </c>
-      <c r="E69" t="s">
-        <v>167</v>
-      </c>
-      <c r="F69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>168</v>
-      </c>
-      <c r="B70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70">
-        <v>2</v>
-      </c>
-      <c r="E70" t="s">
-        <v>169</v>
-      </c>
-      <c r="F70" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>170</v>
-      </c>
-      <c r="B71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C71" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71">
-        <v>2</v>
-      </c>
-      <c r="E71" t="s">
-        <v>171</v>
-      </c>
-      <c r="F71" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>6</v>
-      </c>
-      <c r="B72" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72">
-        <v>2</v>
-      </c>
-      <c r="E72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>11</v>
-      </c>
-      <c r="B73" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73">
-        <v>2</v>
-      </c>
-      <c r="E73" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>16</v>
-      </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74">
-        <v>2</v>
-      </c>
-      <c r="E74" t="s">
-        <v>17</v>
-      </c>
-      <c r="F74" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>18</v>
-      </c>
-      <c r="B75" t="s">
-        <v>12</v>
-      </c>
-      <c r="C75" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75">
-        <v>2</v>
-      </c>
-      <c r="E75" t="s">
-        <v>19</v>
-      </c>
-      <c r="F75" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F77"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="49" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="34" customWidth="1"/>
-    <col min="6" max="6" width="63" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Clean up Script 4, add functions, update README
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B623F58-F9A1-4E6D-8D33-F750EA407D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCFA7E8-AB8E-49A0-B428-9DD30A9FD91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="2710" windowWidth="21600" windowHeight="10950" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Multi-jobs" sheetId="1" r:id="rId1"/>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1186,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" activeCellId="1" sqref="A13:XFD13 A11:XFD11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
README - update description of folders with results for future users to compare to
</commit_message>
<xml_diff>
--- a/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
+++ b/input/Overall_Running_Metadata_for_All_LCMSMS_Jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\LCMSMS_data_analysis_workflow\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCFA7E8-AB8E-49A0-B428-9DD30A9FD91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FE100E-B645-4BB2-B185-868B39931A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="2060" windowWidth="16630" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Multi-jobs" sheetId="1" r:id="rId1"/>
@@ -941,7 +941,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" activeCellId="1" sqref="A13:XFD13 A11:XFD11"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2790,8 +2790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" activeCellId="1" sqref="A13:XFD13 A11:XFD11"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>